<commit_message>
Chỉnh sửa bản cập nhật thông tin
</commit_message>
<xml_diff>
--- a/Thiết kế/Thiết kế giao diện/Phạm Huy Thiết kế/CapNhatThongTinNV.xlsx
+++ b/Thiết kế/Thiết kế giao diện/Phạm Huy Thiết kế/CapNhatThongTinNV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huy/Downloads/CNPM/Thiết kế/Thiết kế giao diện/Phạm Huy Thiết kế/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE57F0D8-8AEF-3B4D-9674-4D780A8ADE35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5EB1F9-8596-794A-B776-9784656BF853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="1120" windowWidth="28040" windowHeight="17440" xr2:uid="{2B64E932-BFF9-7042-8915-7832FAF5A499}"/>
+    <workbookView xWindow="2860" yWindow="2660" windowWidth="28040" windowHeight="17440" xr2:uid="{2B64E932-BFF9-7042-8915-7832FAF5A499}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
   <si>
     <t>Danh sách các biến cố</t>
   </si>
@@ -112,9 +112,6 @@
     <t>RadioBt_GioiTinh</t>
   </si>
   <si>
-    <t>RadioButton</t>
-  </si>
-  <si>
     <t>Chọn giới tính</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>Tf_ViTri</t>
   </si>
   <si>
-    <t>Nhập Vị Trí</t>
-  </si>
-  <si>
     <t>Hiển thị nhãn Mã nhân viên</t>
   </si>
   <si>
@@ -242,6 +236,9 @@
   </si>
   <si>
     <t>huỷ những thông tin vừa nhập</t>
+  </si>
+  <si>
+    <t>Chọn Vị trí</t>
   </si>
 </sst>
 </file>
@@ -981,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C8B081-617A-CE44-8F3A-2769DBFD926B}">
   <dimension ref="A34:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>21</v>
@@ -1132,10 +1129,10 @@
         <v>2</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>23</v>
@@ -1152,10 +1149,10 @@
         <v>24</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -1166,13 +1163,13 @@
         <v>4</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
@@ -1183,13 +1180,13 @@
         <v>5</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -1200,13 +1197,13 @@
         <v>6</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
@@ -1217,18 +1214,18 @@
         <v>7</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -1236,13 +1233,13 @@
         <v>8</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
@@ -1253,13 +1250,13 @@
         <v>9</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
@@ -1270,13 +1267,13 @@
         <v>10</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
@@ -1287,13 +1284,13 @@
         <v>11</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
@@ -1304,13 +1301,13 @@
         <v>12</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -1321,13 +1318,13 @@
         <v>13</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -1338,13 +1335,13 @@
         <v>14</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -1355,13 +1352,13 @@
         <v>15</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -1372,13 +1369,13 @@
         <v>16</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -1389,13 +1386,13 @@
         <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -1406,13 +1403,13 @@
         <v>18</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -1423,13 +1420,13 @@
         <v>19</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
@@ -1440,13 +1437,13 @@
         <v>20</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -1457,13 +1454,13 @@
         <v>21</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>

</xml_diff>